<commit_message>
adjust positive test case
</commit_message>
<xml_diff>
--- a/rules/NEW-RULE/positive/01/data/new-rule-positive-01.xlsx
+++ b/rules/NEW-RULE/positive/01/data/new-rule-positive-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Documents/github/core-contributor/rules/NEW-RULE/positive/01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4E02E5-4377-554E-A412-161EF48C27D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53DF6F1-F8DE-3442-B366-07B1599719C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="pp.xpt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>Product</t>
   </si>
@@ -178,6 +179,18 @@
   </si>
   <si>
     <t>Pharmacokinetics Parameters</t>
+  </si>
+  <si>
+    <t>01-005</t>
+  </si>
+  <si>
+    <t>AURC Infinity Obs Norm by Dose</t>
+  </si>
+  <si>
+    <t>day*ug/mL/mg</t>
+  </si>
+  <si>
+    <t>01-006</t>
   </si>
 </sst>
 </file>
@@ -185,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode=".00"/>
+    <numFmt numFmtId="164" formatCode=".00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -354,7 +367,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -719,13 +732,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68584BE9-C735-0845-AF53-87D093C8EA42}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -962,7 +978,102 @@
         <v>50</v>
       </c>
     </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1194.546</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1195</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1195</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1194.546</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1195</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1195</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>